<commit_message>
Update .xsxl file as Dale updated the Stata version
</commit_message>
<xml_diff>
--- a/Demo_Datasets/ES/Multi-Lingual Phrases - En Fr Es Pt.xlsx
+++ b/Demo_Datasets/ES/Multi-Lingual Phrases - En Fr Es Pt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Dropbox (Biostat Global)\MKT GitHub\vcqi-stata-bgc\LIBRARY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Biostat Global Dropbox\Dale Rhoda\DAR GitHub Repos\vcqi-stata-bgc\LIBRARY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB14471E-4638-439B-8536-6336556CE5F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D645EC-F575-4D95-A37A-7190FB654824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2808" yWindow="2808" windowWidth="17280" windowHeight="9048" xr2:uid="{50234D21-0CB7-4831-B1A7-1E2C296C3191}"/>
+    <workbookView xWindow="5865" yWindow="0" windowWidth="22935" windowHeight="15480" xr2:uid="{50234D21-0CB7-4831-B1A7-1E2C296C3191}"/>
   </bookViews>
   <sheets>
     <sheet name="Latest version" sheetId="1" r:id="rId1"/>
@@ -221,7 +221,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3179" uniqueCount="1916">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3179" uniqueCount="1919">
   <si>
     <t>string_name</t>
   </si>
@@ -5426,9 +5426,6 @@
     <t>Had MOSV for any dose</t>
   </si>
   <si>
-    <t>MOSV and valid doses administered on visit day</t>
-  </si>
-  <si>
     <t>MOSV corrected for</t>
   </si>
   <si>
@@ -6015,6 +6012,18 @@
   </si>
   <si>
     <t>Não forneceu um motivo/sintoma</t>
+  </si>
+  <si>
+    <t>Doses valides reçues le jour de la visite</t>
+  </si>
+  <si>
+    <t>Dosis válidas recibidas en el día de la visita</t>
+  </si>
+  <si>
+    <t>Doses válidas recebidas no dia da visita</t>
+  </si>
+  <si>
+    <t>Valid doses received on visit day</t>
   </si>
 </sst>
 </file>
@@ -6501,19 +6510,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAF4C18C-2D72-4199-BAD0-E065A11CBF01}">
   <dimension ref="A1:AQ384"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A375" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E383" sqref="E383:E384"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="44.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="44.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.83984375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="44.41796875" style="3"/>
-    <col min="3" max="3" width="50.26171875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="54.41796875" style="3" customWidth="1"/>
-    <col min="5" max="43" width="44.41796875" style="4"/>
-    <col min="44" max="16384" width="44.41796875" style="3"/>
+    <col min="1" max="1" width="16.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" style="3"/>
+    <col min="3" max="3" width="50.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="54.42578125" style="3" customWidth="1"/>
+    <col min="5" max="43" width="44.42578125" style="4"/>
+    <col min="44" max="16384" width="44.42578125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1">
@@ -6771,7 +6780,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="16" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A16" s="3" t="s">
         <v>68</v>
       </c>
@@ -6788,7 +6797,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="4" customFormat="1">
+    <row r="17" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A17" s="3" t="s">
         <v>73</v>
       </c>
@@ -7043,7 +7052,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="32" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A32" s="3" t="s">
         <v>148</v>
       </c>
@@ -7060,7 +7069,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="33" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A33" s="3" t="s">
         <v>153</v>
       </c>
@@ -7077,7 +7086,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="34" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A34" s="3" t="s">
         <v>158</v>
       </c>
@@ -7094,7 +7103,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="35" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A35" s="3" t="s">
         <v>163</v>
       </c>
@@ -7145,7 +7154,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="38" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A38" s="3" t="s">
         <v>178</v>
       </c>
@@ -7269,16 +7278,16 @@
         <v>213</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>1719</v>
+        <v>1918</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>215</v>
+        <v>1916</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>216</v>
+        <v>1915</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>217</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="4" customFormat="1">
@@ -7286,7 +7295,7 @@
         <v>218</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>220</v>
@@ -7303,7 +7312,7 @@
         <v>223</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>225</v>
@@ -7320,7 +7329,7 @@
         <v>228</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>230</v>
@@ -7383,7 +7392,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="4" customFormat="1" ht="57.6">
+    <row r="52" spans="1:5" s="4" customFormat="1" ht="60">
       <c r="A52" s="3" t="s">
         <v>245</v>
       </c>
@@ -7400,7 +7409,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="53" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A53" s="3" t="s">
         <v>249</v>
       </c>
@@ -7575,7 +7584,7 @@
         <v>298</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="C63" s="7" t="s">
         <v>300</v>
@@ -7592,7 +7601,7 @@
         <v>303</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>1724</v>
+        <v>1723</v>
       </c>
       <c r="C64" s="7" t="s">
         <v>305</v>
@@ -7609,7 +7618,7 @@
         <v>308</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>1725</v>
+        <v>1724</v>
       </c>
       <c r="C65" s="7" t="s">
         <v>310</v>
@@ -7626,7 +7635,7 @@
         <v>313</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="C66" s="7" t="s">
         <v>315</v>
@@ -7643,7 +7652,7 @@
         <v>318</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="C67" s="7" t="s">
         <v>320</v>
@@ -7660,7 +7669,7 @@
         <v>323</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
       <c r="C68" s="7" t="s">
         <v>325</v>
@@ -7694,7 +7703,7 @@
         <v>333</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>1729</v>
+        <v>1728</v>
       </c>
       <c r="C70" s="7" t="s">
         <v>335</v>
@@ -7723,7 +7732,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="72" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="72" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A72" s="3" t="s">
         <v>343</v>
       </c>
@@ -7740,12 +7749,12 @@
         <v>347</v>
       </c>
     </row>
-    <row r="73" spans="1:5" s="4" customFormat="1">
+    <row r="73" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A73" s="3" t="s">
         <v>348</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="C73" s="7" t="s">
         <v>350</v>
@@ -7791,7 +7800,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="76" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="76" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A76" s="3" t="s">
         <v>361</v>
       </c>
@@ -7808,7 +7817,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="77" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="77" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A77" s="3" t="s">
         <v>366</v>
       </c>
@@ -7825,7 +7834,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="78" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="78" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A78" s="3" t="s">
         <v>371</v>
       </c>
@@ -7842,7 +7851,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="79" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="79" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A79" s="3" t="s">
         <v>375</v>
       </c>
@@ -7859,7 +7868,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="80" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="80" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A80" s="3" t="s">
         <v>380</v>
       </c>
@@ -7898,7 +7907,7 @@
         <v>388</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="C82" s="7" t="s">
         <v>390</v>
@@ -7915,7 +7924,7 @@
         <v>393</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="C83" s="7" t="s">
         <v>395</v>
@@ -8012,7 +8021,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="89" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="89" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A89" s="3" t="s">
         <v>423</v>
       </c>
@@ -8029,7 +8038,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="90" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="90" spans="1:5" s="4" customFormat="1" ht="60">
       <c r="A90" s="3" t="s">
         <v>428</v>
       </c>
@@ -8046,7 +8055,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="91" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="91" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A91" s="3" t="s">
         <v>433</v>
       </c>
@@ -8148,7 +8157,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="97" spans="1:5" s="4" customFormat="1">
+    <row r="97" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A97" s="3" t="s">
         <v>463</v>
       </c>
@@ -8233,7 +8242,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="102" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="102" spans="1:5" s="4" customFormat="1" ht="60">
       <c r="A102" s="3" t="s">
         <v>488</v>
       </c>
@@ -8301,7 +8310,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="106" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="106" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A106" s="3" t="s">
         <v>508</v>
       </c>
@@ -8318,7 +8327,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="107" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="107" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A107" s="3" t="s">
         <v>513</v>
       </c>
@@ -8335,7 +8344,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="108" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="108" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A108" s="3" t="s">
         <v>518</v>
       </c>
@@ -8352,7 +8361,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="109" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="109" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A109" s="3" t="s">
         <v>523</v>
       </c>
@@ -8369,7 +8378,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="110" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="110" spans="1:5" s="4" customFormat="1" ht="60">
       <c r="A110" s="3" t="s">
         <v>528</v>
       </c>
@@ -8386,7 +8395,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="111" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="111" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A111" s="3" t="s">
         <v>533</v>
       </c>
@@ -8403,7 +8412,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="112" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="112" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A112" s="3" t="s">
         <v>538</v>
       </c>
@@ -8420,7 +8429,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="113" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="113" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A113" s="3" t="s">
         <v>543</v>
       </c>
@@ -8437,7 +8446,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="114" spans="1:5" s="4" customFormat="1">
+    <row r="114" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A114" s="3" t="s">
         <v>548</v>
       </c>
@@ -8454,7 +8463,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="115" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="115" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A115" s="3" t="s">
         <v>553</v>
       </c>
@@ -8590,12 +8599,12 @@
         <v>592</v>
       </c>
     </row>
-    <row r="123" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="123" spans="1:5" s="4" customFormat="1" ht="60">
       <c r="A123" s="3" t="s">
         <v>593</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="C123" s="7" t="s">
         <v>595</v>
@@ -8663,7 +8672,7 @@
         <v>613</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
       <c r="C127" s="7" t="s">
         <v>615</v>
@@ -8692,12 +8701,12 @@
         <v>622</v>
       </c>
     </row>
-    <row r="129" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="129" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A129" s="3" t="s">
         <v>623</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="C129" s="7" t="s">
         <v>625</v>
@@ -8743,7 +8752,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="132" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="132" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A132" s="3" t="s">
         <v>638</v>
       </c>
@@ -8760,7 +8769,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="133" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="133" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A133" s="3" t="s">
         <v>643</v>
       </c>
@@ -8777,7 +8786,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="134" spans="1:5" s="4" customFormat="1" ht="72">
+    <row r="134" spans="1:5" s="4" customFormat="1" ht="75">
       <c r="A134" s="3" t="s">
         <v>648</v>
       </c>
@@ -8799,7 +8808,7 @@
         <v>653</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="C135" s="7" t="s">
         <v>655</v>
@@ -8845,7 +8854,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="138" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="138" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A138" s="3" t="s">
         <v>668</v>
       </c>
@@ -8862,7 +8871,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="139" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="139" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A139" s="3" t="s">
         <v>673</v>
       </c>
@@ -8879,7 +8888,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="140" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="140" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A140" s="3" t="s">
         <v>678</v>
       </c>
@@ -8896,12 +8905,12 @@
         <v>682</v>
       </c>
     </row>
-    <row r="141" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="141" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A141" s="3" t="s">
         <v>683</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="C141" s="9" t="s">
         <v>685</v>
@@ -8930,12 +8939,12 @@
         <v>692</v>
       </c>
     </row>
-    <row r="143" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="143" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A143" s="3" t="s">
         <v>693</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="C143" s="7" t="s">
         <v>695</v>
@@ -8947,7 +8956,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="144" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="144" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A144" s="3" t="s">
         <v>698</v>
       </c>
@@ -8969,7 +8978,7 @@
         <v>703</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="C145" s="7" t="s">
         <v>705</v>
@@ -8986,7 +8995,7 @@
         <v>708</v>
       </c>
       <c r="B146" s="6" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="C146" s="7" t="s">
         <v>710</v>
@@ -9003,7 +9012,7 @@
         <v>713</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="C147" s="7" t="s">
         <v>715</v>
@@ -9015,7 +9024,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="148" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="148" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A148" s="3" t="s">
         <v>718</v>
       </c>
@@ -9032,12 +9041,12 @@
         <v>722</v>
       </c>
     </row>
-    <row r="149" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="149" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A149" s="3" t="s">
         <v>723</v>
       </c>
       <c r="B149" s="6" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="C149" s="7" t="s">
         <v>725</v>
@@ -9054,7 +9063,7 @@
         <v>728</v>
       </c>
       <c r="B150" s="6" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="C150" s="7" t="s">
         <v>730</v>
@@ -9066,7 +9075,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="151" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="151" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A151" s="3" t="s">
         <v>733</v>
       </c>
@@ -9100,7 +9109,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="153" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="153" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A153" s="3" t="s">
         <v>743</v>
       </c>
@@ -9117,7 +9126,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="154" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="154" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A154" s="3" t="s">
         <v>748</v>
       </c>
@@ -9134,7 +9143,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="155" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="155" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A155" s="3" t="s">
         <v>753</v>
       </c>
@@ -9151,12 +9160,12 @@
         <v>757</v>
       </c>
     </row>
-    <row r="156" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="156" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A156" s="3" t="s">
         <v>758</v>
       </c>
       <c r="B156" s="6" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="C156" s="7" t="s">
         <v>760</v>
@@ -9168,7 +9177,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="157" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="157" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A157" s="3" t="s">
         <v>763</v>
       </c>
@@ -9202,7 +9211,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="159" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="159" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A159" s="3" t="s">
         <v>773</v>
       </c>
@@ -9236,12 +9245,12 @@
         <v>782</v>
       </c>
     </row>
-    <row r="161" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="161" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A161" s="3" t="s">
         <v>783</v>
       </c>
       <c r="B161" s="6" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="C161" s="7" t="s">
         <v>785</v>
@@ -9253,7 +9262,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="162" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="162" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A162" s="3" t="s">
         <v>788</v>
       </c>
@@ -9270,12 +9279,12 @@
         <v>792</v>
       </c>
     </row>
-    <row r="163" spans="1:5" s="4" customFormat="1" ht="57.6">
+    <row r="163" spans="1:5" s="4" customFormat="1" ht="60">
       <c r="A163" s="3" t="s">
         <v>793</v>
       </c>
       <c r="B163" s="6" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="C163" s="9" t="s">
         <v>795</v>
@@ -9287,12 +9296,12 @@
         <v>797</v>
       </c>
     </row>
-    <row r="164" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="164" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A164" s="3" t="s">
         <v>798</v>
       </c>
       <c r="B164" s="6" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="C164" s="7" t="s">
         <v>800</v>
@@ -9309,7 +9318,7 @@
         <v>803</v>
       </c>
       <c r="B165" s="6" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="C165" s="7" t="s">
         <v>805</v>
@@ -9321,7 +9330,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="166" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="166" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A166" s="3" t="s">
         <v>808</v>
       </c>
@@ -9338,12 +9347,12 @@
         <v>812</v>
       </c>
     </row>
-    <row r="167" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="167" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A167" s="3" t="s">
         <v>813</v>
       </c>
       <c r="B167" s="6" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="C167" s="7" t="s">
         <v>815</v>
@@ -9360,7 +9369,7 @@
         <v>818</v>
       </c>
       <c r="B168" s="6" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="C168" s="7" t="s">
         <v>820</v>
@@ -9372,7 +9381,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="169" spans="1:5" s="4" customFormat="1" ht="57.6">
+    <row r="169" spans="1:5" s="4" customFormat="1" ht="75">
       <c r="A169" s="3" t="s">
         <v>823</v>
       </c>
@@ -9389,12 +9398,12 @@
         <v>827</v>
       </c>
     </row>
-    <row r="170" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="170" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A170" s="3" t="s">
         <v>828</v>
       </c>
       <c r="B170" s="6" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="C170" s="7" t="s">
         <v>830</v>
@@ -9406,12 +9415,12 @@
         <v>832</v>
       </c>
     </row>
-    <row r="171" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="171" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A171" s="3" t="s">
         <v>833</v>
       </c>
       <c r="B171" s="6" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="C171" s="7" t="s">
         <v>835</v>
@@ -9423,12 +9432,12 @@
         <v>837</v>
       </c>
     </row>
-    <row r="172" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="172" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A172" s="3" t="s">
         <v>838</v>
       </c>
       <c r="B172" s="6" t="s">
-        <v>1753</v>
+        <v>1752</v>
       </c>
       <c r="C172" s="7" t="s">
         <v>840</v>
@@ -9440,12 +9449,12 @@
         <v>842</v>
       </c>
     </row>
-    <row r="173" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="173" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A173" s="3" t="s">
         <v>843</v>
       </c>
       <c r="B173" s="6" t="s">
-        <v>1754</v>
+        <v>1753</v>
       </c>
       <c r="C173" s="7" t="s">
         <v>845</v>
@@ -9462,7 +9471,7 @@
         <v>848</v>
       </c>
       <c r="B174" s="6" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="C174" s="9" t="s">
         <v>850</v>
@@ -9508,7 +9517,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="177" spans="1:5" s="4" customFormat="1">
+    <row r="177" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A177" s="3" t="s">
         <v>863</v>
       </c>
@@ -9525,7 +9534,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="178" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="178" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A178" s="3" t="s">
         <v>868</v>
       </c>
@@ -9559,7 +9568,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="180" spans="1:5" s="4" customFormat="1" ht="57.6">
+    <row r="180" spans="1:5" s="4" customFormat="1" ht="75">
       <c r="A180" s="3" t="s">
         <v>878</v>
       </c>
@@ -9593,7 +9602,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="182" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="182" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A182" s="3" t="s">
         <v>888</v>
       </c>
@@ -9610,7 +9619,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="183" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="183" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A183" s="3" t="s">
         <v>893</v>
       </c>
@@ -9644,7 +9653,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="185" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="185" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A185" s="3" t="s">
         <v>903</v>
       </c>
@@ -9678,7 +9687,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="187" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="187" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A187" s="3" t="s">
         <v>913</v>
       </c>
@@ -9695,7 +9704,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="188" spans="1:5" s="4" customFormat="1" ht="115.2">
+    <row r="188" spans="1:5" s="4" customFormat="1" ht="135">
       <c r="A188" s="3" t="s">
         <v>918</v>
       </c>
@@ -9712,7 +9721,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="189" spans="1:5" s="4" customFormat="1" ht="72">
+    <row r="189" spans="1:5" s="4" customFormat="1" ht="75">
       <c r="A189" s="3" t="s">
         <v>923</v>
       </c>
@@ -9729,7 +9738,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="190" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="190" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A190" s="3" t="s">
         <v>928</v>
       </c>
@@ -9746,7 +9755,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="191" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="191" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A191" s="3" t="s">
         <v>933</v>
       </c>
@@ -9763,7 +9772,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="192" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="192" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A192" s="3" t="s">
         <v>938</v>
       </c>
@@ -9780,7 +9789,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="193" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="193" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A193" s="3" t="s">
         <v>943</v>
       </c>
@@ -9797,7 +9806,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="194" spans="1:5" s="4" customFormat="1" ht="100.8">
+    <row r="194" spans="1:5" s="4" customFormat="1" ht="105">
       <c r="A194" s="3" t="s">
         <v>948</v>
       </c>
@@ -9814,7 +9823,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="195" spans="1:5" s="4" customFormat="1" ht="86.4">
+    <row r="195" spans="1:5" s="4" customFormat="1" ht="105">
       <c r="A195" s="3" t="s">
         <v>953</v>
       </c>
@@ -9831,7 +9840,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="196" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="196" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A196" s="3" t="s">
         <v>958</v>
       </c>
@@ -9848,7 +9857,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="197" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="197" spans="1:5" s="4" customFormat="1" ht="60">
       <c r="A197" s="3" t="s">
         <v>963</v>
       </c>
@@ -9865,7 +9874,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="198" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="198" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A198" s="3" t="s">
         <v>968</v>
       </c>
@@ -9887,7 +9896,7 @@
         <v>973</v>
       </c>
       <c r="B199" s="6" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
       <c r="C199" s="7" t="s">
         <v>975</v>
@@ -9904,7 +9913,7 @@
         <v>978</v>
       </c>
       <c r="B200" s="6" t="s">
-        <v>1757</v>
+        <v>1756</v>
       </c>
       <c r="C200" s="7" t="s">
         <v>980</v>
@@ -9916,12 +9925,12 @@
         <v>982</v>
       </c>
     </row>
-    <row r="201" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="201" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A201" s="3" t="s">
         <v>983</v>
       </c>
       <c r="B201" s="6" t="s">
-        <v>1758</v>
+        <v>1757</v>
       </c>
       <c r="C201" s="7" t="s">
         <v>985</v>
@@ -10001,7 +10010,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="206" spans="1:5" s="4" customFormat="1">
+    <row r="206" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A206" s="3" t="s">
         <v>1008</v>
       </c>
@@ -10018,7 +10027,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="207" spans="1:5" s="4" customFormat="1">
+    <row r="207" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A207" s="3" t="s">
         <v>1013</v>
       </c>
@@ -10052,7 +10061,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="209" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="209" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A209" s="3" t="s">
         <v>1023</v>
       </c>
@@ -10069,7 +10078,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="210" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="210" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A210" s="3" t="s">
         <v>1028</v>
       </c>
@@ -10086,7 +10095,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="211" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="211" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A211" s="3" t="s">
         <v>1033</v>
       </c>
@@ -10120,7 +10129,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="213" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="213" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A213" s="3" t="s">
         <v>1043</v>
       </c>
@@ -10137,7 +10146,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="214" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="214" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A214" s="3" t="s">
         <v>1048</v>
       </c>
@@ -10154,7 +10163,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="215" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="215" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A215" s="3" t="s">
         <v>1053</v>
       </c>
@@ -10171,7 +10180,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="216" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="216" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A216" s="3" t="s">
         <v>1058</v>
       </c>
@@ -10188,7 +10197,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="217" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="217" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A217" s="3" t="s">
         <v>1063</v>
       </c>
@@ -10346,7 +10355,7 @@
         <v>1108</v>
       </c>
       <c r="B226" s="6" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="C226" s="7" t="s">
         <v>95</v>
@@ -10358,12 +10367,12 @@
         <v>97</v>
       </c>
     </row>
-    <row r="227" spans="1:5" s="4" customFormat="1">
+    <row r="227" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A227" s="3" t="s">
         <v>1111</v>
       </c>
       <c r="B227" s="6" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="C227" s="7" t="s">
         <v>1113</v>
@@ -10380,7 +10389,7 @@
         <v>1116</v>
       </c>
       <c r="B228" s="6" t="s">
-        <v>1761</v>
+        <v>1760</v>
       </c>
       <c r="C228" s="7" t="s">
         <v>1118</v>
@@ -10397,7 +10406,7 @@
         <v>1121</v>
       </c>
       <c r="B229" s="6" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
       <c r="C229" s="7" t="s">
         <v>1123</v>
@@ -10414,7 +10423,7 @@
         <v>1126</v>
       </c>
       <c r="B230" s="6" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
       <c r="C230" s="7" t="s">
         <v>1128</v>
@@ -10448,7 +10457,7 @@
         <v>1136</v>
       </c>
       <c r="B232" s="6" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
       <c r="C232" s="7" t="s">
         <v>1138</v>
@@ -10460,7 +10469,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="233" spans="1:5" s="4" customFormat="1" ht="43" customHeight="1">
+    <row r="233" spans="1:5" s="4" customFormat="1" ht="42.95" customHeight="1">
       <c r="A233" s="3" t="s">
         <v>1141</v>
       </c>
@@ -10477,7 +10486,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="234" spans="1:5" s="4" customFormat="1">
+    <row r="234" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A234" s="3" t="s">
         <v>1146</v>
       </c>
@@ -10511,7 +10520,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="236" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="236" spans="1:5" s="4" customFormat="1" ht="60">
       <c r="A236" s="3" t="s">
         <v>1156</v>
       </c>
@@ -10528,7 +10537,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="237" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="237" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A237" s="3" t="s">
         <v>1160</v>
       </c>
@@ -10562,7 +10571,7 @@
         <v>1169</v>
       </c>
     </row>
-    <row r="239" spans="1:5" s="4" customFormat="1">
+    <row r="239" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A239" s="3" t="s">
         <v>1170</v>
       </c>
@@ -10579,7 +10588,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="240" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="240" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A240" s="3" t="s">
         <v>1175</v>
       </c>
@@ -10647,7 +10656,7 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="244" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="244" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A244" s="3" t="s">
         <v>1195</v>
       </c>
@@ -10664,7 +10673,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="245" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="245" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A245" s="3" t="s">
         <v>1200</v>
       </c>
@@ -10681,7 +10690,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="246" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="246" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A246" s="3" t="s">
         <v>1205</v>
       </c>
@@ -10715,7 +10724,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="248" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="248" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A248" s="3" t="s">
         <v>1215</v>
       </c>
@@ -10732,7 +10741,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="249" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="249" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A249" s="3" t="s">
         <v>1220</v>
       </c>
@@ -11208,7 +11217,7 @@
         <v>1356</v>
       </c>
     </row>
-    <row r="277" spans="1:5" ht="28.8">
+    <row r="277" spans="1:5" ht="30">
       <c r="A277" s="3" t="s">
         <v>1358</v>
       </c>
@@ -11327,7 +11336,7 @@
         <v>1418</v>
       </c>
     </row>
-    <row r="284" spans="1:5">
+    <row r="284" spans="1:5" ht="30">
       <c r="A284" s="3" t="s">
         <v>1386</v>
       </c>
@@ -11344,7 +11353,7 @@
         <v>1424</v>
       </c>
     </row>
-    <row r="285" spans="1:5">
+    <row r="285" spans="1:5" ht="30">
       <c r="A285" s="3" t="s">
         <v>1387</v>
       </c>
@@ -11446,7 +11455,7 @@
         <v>1452</v>
       </c>
     </row>
-    <row r="291" spans="1:5" ht="28.8">
+    <row r="291" spans="1:5" ht="30">
       <c r="A291" s="3" t="s">
         <v>1393</v>
       </c>
@@ -11480,7 +11489,7 @@
         <v>1458</v>
       </c>
     </row>
-    <row r="293" spans="1:5" ht="28.8">
+    <row r="293" spans="1:5" ht="30">
       <c r="A293" s="3" t="s">
         <v>1395</v>
       </c>
@@ -11514,7 +11523,7 @@
         <v>1464</v>
       </c>
     </row>
-    <row r="295" spans="1:5" ht="28.8">
+    <row r="295" spans="1:5" ht="30">
       <c r="A295" s="3" t="s">
         <v>1397</v>
       </c>
@@ -12024,7 +12033,7 @@
         <v>1592</v>
       </c>
     </row>
-    <row r="325" spans="1:5" ht="28.8">
+    <row r="325" spans="1:5" ht="30">
       <c r="A325" s="3" t="s">
         <v>1495</v>
       </c>
@@ -12041,7 +12050,7 @@
         <v>1655</v>
       </c>
     </row>
-    <row r="326" spans="1:5" ht="28.8">
+    <row r="326" spans="1:5" ht="30">
       <c r="A326" s="3" t="s">
         <v>1496</v>
       </c>
@@ -12092,7 +12101,7 @@
         <v>1658</v>
       </c>
     </row>
-    <row r="329" spans="1:5" ht="28.8">
+    <row r="329" spans="1:5" ht="30">
       <c r="A329" s="3" t="s">
         <v>1499</v>
       </c>
@@ -12109,7 +12118,7 @@
         <v>1659</v>
       </c>
     </row>
-    <row r="330" spans="1:5" ht="28.8">
+    <row r="330" spans="1:5" ht="30">
       <c r="A330" s="3" t="s">
         <v>1500</v>
       </c>
@@ -12126,7 +12135,7 @@
         <v>1660</v>
       </c>
     </row>
-    <row r="331" spans="1:5" ht="28.8">
+    <row r="331" spans="1:5" ht="45">
       <c r="A331" s="3" t="s">
         <v>1501</v>
       </c>
@@ -12143,7 +12152,7 @@
         <v>1661</v>
       </c>
     </row>
-    <row r="332" spans="1:5" ht="43.2">
+    <row r="332" spans="1:5" ht="45">
       <c r="A332" s="3" t="s">
         <v>1502</v>
       </c>
@@ -12160,7 +12169,7 @@
         <v>1662</v>
       </c>
     </row>
-    <row r="333" spans="1:5" ht="28.8">
+    <row r="333" spans="1:5" ht="45">
       <c r="A333" s="3" t="s">
         <v>1503</v>
       </c>
@@ -12177,7 +12186,7 @@
         <v>1663</v>
       </c>
     </row>
-    <row r="334" spans="1:5">
+    <row r="334" spans="1:5" ht="30">
       <c r="A334" s="3" t="s">
         <v>1504</v>
       </c>
@@ -12233,7 +12242,7 @@
         <v>1507</v>
       </c>
       <c r="B337" s="11" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="C337" s="11" t="s">
         <v>1606</v>
@@ -12245,7 +12254,7 @@
         <v>1607</v>
       </c>
     </row>
-    <row r="338" spans="1:6" ht="57.6">
+    <row r="338" spans="1:6" ht="60">
       <c r="A338" s="3" t="s">
         <v>1508</v>
       </c>
@@ -12262,24 +12271,24 @@
         <v>1667</v>
       </c>
     </row>
-    <row r="339" spans="1:6" ht="57.6">
+    <row r="339" spans="1:6" ht="60">
       <c r="A339" s="3" t="s">
         <v>1509</v>
       </c>
       <c r="B339" s="11" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="C339" s="11" t="s">
+        <v>1870</v>
+      </c>
+      <c r="D339" s="11" t="s">
         <v>1871</v>
       </c>
-      <c r="D339" s="11" t="s">
+      <c r="E339" s="11" t="s">
         <v>1872</v>
       </c>
-      <c r="E339" s="11" t="s">
-        <v>1873</v>
-      </c>
-    </row>
-    <row r="340" spans="1:6" ht="26.1">
+    </row>
+    <row r="340" spans="1:6" ht="30">
       <c r="A340" s="3" t="s">
         <v>1510</v>
       </c>
@@ -12297,7 +12306,7 @@
       </c>
       <c r="F340" s="14"/>
     </row>
-    <row r="341" spans="1:6" ht="28.8">
+    <row r="341" spans="1:6" ht="30">
       <c r="A341" s="3" t="s">
         <v>1511</v>
       </c>
@@ -12314,7 +12323,7 @@
         <v>1684</v>
       </c>
     </row>
-    <row r="342" spans="1:6" ht="28.8">
+    <row r="342" spans="1:6" ht="30">
       <c r="A342" s="3" t="s">
         <v>1512</v>
       </c>
@@ -12331,7 +12340,7 @@
         <v>1648</v>
       </c>
     </row>
-    <row r="343" spans="1:6" ht="28.8">
+    <row r="343" spans="1:6" ht="30">
       <c r="A343" s="3" t="s">
         <v>1513</v>
       </c>
@@ -12348,7 +12357,7 @@
         <v>1649</v>
       </c>
     </row>
-    <row r="344" spans="1:6" ht="28.8">
+    <row r="344" spans="1:6" ht="30">
       <c r="A344" s="3" t="s">
         <v>1514</v>
       </c>
@@ -12382,7 +12391,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="346" spans="1:6" ht="28.8">
+    <row r="346" spans="1:6" ht="30">
       <c r="A346" s="3" t="s">
         <v>1516</v>
       </c>
@@ -12416,7 +12425,7 @@
         <v>1653</v>
       </c>
     </row>
-    <row r="348" spans="1:6" ht="28.8">
+    <row r="348" spans="1:6" ht="30">
       <c r="A348" s="3" t="s">
         <v>1518</v>
       </c>
@@ -12509,13 +12518,13 @@
         <v>1708</v>
       </c>
       <c r="C353" s="15" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="D353" s="15" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="E353" s="15" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
     </row>
     <row r="354" spans="1:5">
@@ -12526,13 +12535,13 @@
         <v>1709</v>
       </c>
       <c r="C354" s="15" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="D354" s="15" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="E354" s="15" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
     </row>
     <row r="355" spans="1:5">
@@ -12543,506 +12552,506 @@
         <v>1710</v>
       </c>
       <c r="C355" s="15" t="s">
-        <v>1776</v>
+        <v>1775</v>
       </c>
       <c r="D355" s="15" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="E355" s="15" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
     </row>
     <row r="356" spans="1:5">
       <c r="A356" s="3" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
       <c r="C356" s="1" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
       <c r="D356" s="1" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
       <c r="E356" s="1" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
     </row>
     <row r="357" spans="1:5">
       <c r="A357" s="3" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="B357" s="15" t="s">
-        <v>1783</v>
+        <v>1782</v>
       </c>
       <c r="C357" s="15" t="s">
-        <v>1808</v>
+        <v>1807</v>
       </c>
       <c r="D357" s="15" t="s">
-        <v>1817</v>
+        <v>1816</v>
       </c>
       <c r="E357" s="15" t="s">
-        <v>1826</v>
+        <v>1825</v>
       </c>
     </row>
     <row r="358" spans="1:5">
       <c r="A358" s="3" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
       <c r="B358" s="15" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="C358" s="15" t="s">
-        <v>1809</v>
+        <v>1808</v>
       </c>
       <c r="D358" s="15" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
       <c r="E358" s="15" t="s">
-        <v>1827</v>
+        <v>1826</v>
       </c>
     </row>
     <row r="359" spans="1:5">
       <c r="A359" s="3" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
       <c r="B359" s="15" t="s">
-        <v>1788</v>
+        <v>1787</v>
       </c>
       <c r="C359" s="15" t="s">
-        <v>1810</v>
+        <v>1809</v>
       </c>
       <c r="D359" s="15" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
       <c r="E359" s="15" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="360" spans="1:5">
       <c r="A360" s="3" t="s">
+        <v>1789</v>
+      </c>
+      <c r="B360" s="15" t="s">
+        <v>1788</v>
+      </c>
+      <c r="C360" s="15" t="s">
+        <v>1810</v>
+      </c>
+      <c r="D360" s="15" t="s">
+        <v>1819</v>
+      </c>
+      <c r="E360" s="15" t="s">
+        <v>1828</v>
+      </c>
+    </row>
+    <row r="361" spans="1:5" ht="30">
+      <c r="A361" s="3" t="s">
         <v>1790</v>
       </c>
-      <c r="B360" s="15" t="s">
-        <v>1789</v>
-      </c>
-      <c r="C360" s="15" t="s">
+      <c r="B361" s="15" t="s">
+        <v>1800</v>
+      </c>
+      <c r="C361" s="15" t="s">
         <v>1811</v>
       </c>
-      <c r="D360" s="15" t="s">
+      <c r="D361" s="15" t="s">
         <v>1820</v>
       </c>
-      <c r="E360" s="15" t="s">
+      <c r="E361" s="15" t="s">
         <v>1829</v>
-      </c>
-    </row>
-    <row r="361" spans="1:5" ht="28.8">
-      <c r="A361" s="3" t="s">
-        <v>1791</v>
-      </c>
-      <c r="B361" s="15" t="s">
-        <v>1801</v>
-      </c>
-      <c r="C361" s="15" t="s">
-        <v>1812</v>
-      </c>
-      <c r="D361" s="15" t="s">
-        <v>1821</v>
-      </c>
-      <c r="E361" s="15" t="s">
-        <v>1830</v>
       </c>
     </row>
     <row r="362" spans="1:5">
       <c r="A362" s="3" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="B362" s="15" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="C362" s="15" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
       <c r="D362" s="15" t="s">
-        <v>1822</v>
+        <v>1821</v>
       </c>
       <c r="E362" s="15" t="s">
-        <v>1831</v>
+        <v>1830</v>
       </c>
     </row>
     <row r="363" spans="1:5">
       <c r="A363" s="3" t="s">
-        <v>1793</v>
+        <v>1792</v>
       </c>
       <c r="B363" s="15" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="C363" s="15" t="s">
-        <v>1814</v>
+        <v>1813</v>
       </c>
       <c r="D363" s="15" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
       <c r="E363" s="15" t="s">
-        <v>1832</v>
+        <v>1831</v>
       </c>
     </row>
     <row r="364" spans="1:5">
       <c r="A364" s="3" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="B364" s="15" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
       <c r="C364" s="15" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
       <c r="D364" s="15" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
       <c r="E364" s="15" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="365" spans="1:5">
       <c r="A365" s="3" t="s">
-        <v>1795</v>
+        <v>1794</v>
       </c>
       <c r="B365" s="15" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="C365" s="15" t="s">
-        <v>1816</v>
+        <v>1815</v>
       </c>
       <c r="D365" s="15" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="E365" s="15" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="366" spans="1:5">
       <c r="A366" s="3" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="C366" s="1" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="D366" s="1" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="E366" s="1" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
     </row>
     <row r="367" spans="1:5">
       <c r="A367" s="3" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
       <c r="B367" s="15" t="s">
-        <v>1835</v>
+        <v>1834</v>
       </c>
       <c r="C367" s="15" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
       <c r="D367" s="15" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
       <c r="E367" s="15" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
     </row>
     <row r="368" spans="1:5">
       <c r="A368" s="3" t="s">
-        <v>1798</v>
+        <v>1797</v>
       </c>
       <c r="B368" s="15" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
       <c r="C368" s="15" t="s">
-        <v>1846</v>
+        <v>1845</v>
       </c>
       <c r="D368" s="15" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="E368" s="15" t="s">
-        <v>1860</v>
+        <v>1859</v>
       </c>
     </row>
     <row r="369" spans="1:5">
       <c r="A369" s="3" t="s">
-        <v>1799</v>
+        <v>1798</v>
       </c>
       <c r="B369" s="15" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
       <c r="C369" s="15" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
       <c r="D369" s="15" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="E369" s="15" t="s">
-        <v>1861</v>
+        <v>1860</v>
       </c>
     </row>
     <row r="370" spans="1:5">
       <c r="A370" s="3" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="B370" s="15" t="s">
+        <v>1837</v>
+      </c>
+      <c r="C370" s="15" t="s">
+        <v>1847</v>
+      </c>
+      <c r="D370" s="15" t="s">
+        <v>1854</v>
+      </c>
+      <c r="E370" s="15" t="s">
+        <v>1861</v>
+      </c>
+    </row>
+    <row r="371" spans="1:5" ht="30">
+      <c r="A371" s="3" t="s">
+        <v>1839</v>
+      </c>
+      <c r="B371" s="15" t="s">
         <v>1838</v>
       </c>
-      <c r="C370" s="15" t="s">
+      <c r="C371" s="15" t="s">
         <v>1848</v>
       </c>
-      <c r="D370" s="15" t="s">
+      <c r="D371" s="15" t="s">
         <v>1855</v>
       </c>
-      <c r="E370" s="15" t="s">
+      <c r="E371" s="15" t="s">
         <v>1862</v>
       </c>
     </row>
-    <row r="371" spans="1:5">
-      <c r="A371" s="3" t="s">
+    <row r="372" spans="1:5" ht="30">
+      <c r="A372" s="3" t="s">
         <v>1840</v>
       </c>
-      <c r="B371" s="15" t="s">
-        <v>1839</v>
-      </c>
-      <c r="C371" s="15" t="s">
+      <c r="B372" s="15" t="s">
+        <v>1842</v>
+      </c>
+      <c r="C372" s="15" t="s">
         <v>1849</v>
       </c>
-      <c r="D371" s="15" t="s">
+      <c r="D372" s="15" t="s">
         <v>1856</v>
       </c>
-      <c r="E371" s="15" t="s">
+      <c r="E372" s="15" t="s">
         <v>1863</v>
       </c>
     </row>
-    <row r="372" spans="1:5" ht="28.8">
-      <c r="A372" s="3" t="s">
+    <row r="373" spans="1:5" ht="30">
+      <c r="A373" s="3" t="s">
         <v>1841</v>
       </c>
-      <c r="B372" s="15" t="s">
+      <c r="B373" s="15" t="s">
         <v>1843</v>
       </c>
-      <c r="C372" s="15" t="s">
+      <c r="C373" s="15" t="s">
         <v>1850</v>
       </c>
-      <c r="D372" s="15" t="s">
+      <c r="D373" s="15" t="s">
         <v>1857</v>
       </c>
-      <c r="E372" s="15" t="s">
+      <c r="E373" s="15" t="s">
         <v>1864</v>
-      </c>
-    </row>
-    <row r="373" spans="1:5">
-      <c r="A373" s="3" t="s">
-        <v>1842</v>
-      </c>
-      <c r="B373" s="15" t="s">
-        <v>1844</v>
-      </c>
-      <c r="C373" s="15" t="s">
-        <v>1851</v>
-      </c>
-      <c r="D373" s="15" t="s">
-        <v>1858</v>
-      </c>
-      <c r="E373" s="15" t="s">
-        <v>1865</v>
       </c>
     </row>
     <row r="374" spans="1:5">
       <c r="A374" s="3" t="s">
+        <v>1865</v>
+      </c>
+      <c r="B374" s="1" t="s">
         <v>1866</v>
       </c>
-      <c r="B374" s="1" t="s">
-        <v>1867</v>
-      </c>
       <c r="C374" s="1" t="s">
-        <v>1867</v>
+        <v>1866</v>
       </c>
       <c r="D374" s="1" t="s">
-        <v>1867</v>
+        <v>1866</v>
       </c>
       <c r="E374" s="2" t="s">
-        <v>1867</v>
+        <v>1866</v>
       </c>
     </row>
     <row r="375" spans="1:5">
       <c r="A375" s="3" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="C375" s="1" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="D375" s="1" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="E375" s="1" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
     </row>
     <row r="376" spans="1:5">
       <c r="A376" s="3" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="B376" s="15" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="C376" s="15" t="s">
-        <v>1890</v>
+        <v>1889</v>
       </c>
       <c r="D376" s="15" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="E376" s="15" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="377" spans="1:5">
       <c r="A377" s="3" t="s">
-        <v>1876</v>
+        <v>1875</v>
       </c>
       <c r="B377" s="15" t="s">
+        <v>1877</v>
+      </c>
+      <c r="C377" s="15" t="s">
         <v>1878</v>
       </c>
-      <c r="C377" s="15" t="s">
+      <c r="D377" s="15" t="s">
         <v>1879</v>
       </c>
-      <c r="D377" s="15" t="s">
-        <v>1880</v>
-      </c>
       <c r="E377" s="15" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
     </row>
     <row r="378" spans="1:5">
       <c r="A378" s="3" t="s">
-        <v>1877</v>
+        <v>1876</v>
       </c>
       <c r="B378" s="15" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="C378" s="15" t="s">
-        <v>1891</v>
+        <v>1890</v>
       </c>
       <c r="D378" s="15" t="s">
-        <v>1897</v>
+        <v>1896</v>
       </c>
       <c r="E378" s="15" t="s">
-        <v>1902</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="379" spans="1:5">
       <c r="A379" s="3" t="s">
-        <v>1883</v>
+        <v>1882</v>
       </c>
       <c r="B379" s="15" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
       <c r="C379" s="15" t="s">
-        <v>1892</v>
+        <v>1891</v>
       </c>
       <c r="D379" s="15" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="E379" s="15" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="380" spans="1:5">
       <c r="A380" s="3" t="s">
+        <v>1884</v>
+      </c>
+      <c r="B380" s="15" t="s">
+        <v>1883</v>
+      </c>
+      <c r="C380" s="15" t="s">
+        <v>1892</v>
+      </c>
+      <c r="D380" s="15" t="s">
+        <v>1898</v>
+      </c>
+      <c r="E380" s="15" t="s">
+        <v>1883</v>
+      </c>
+    </row>
+    <row r="381" spans="1:5" ht="30">
+      <c r="A381" s="3" t="s">
         <v>1885</v>
       </c>
-      <c r="B380" s="15" t="s">
-        <v>1884</v>
-      </c>
-      <c r="C380" s="15" t="s">
+      <c r="B381" s="15" t="s">
+        <v>1886</v>
+      </c>
+      <c r="C381" s="15" t="s">
         <v>1893</v>
       </c>
-      <c r="D380" s="15" t="s">
+      <c r="D381" s="15" t="s">
         <v>1899</v>
       </c>
-      <c r="E380" s="15" t="s">
-        <v>1884</v>
-      </c>
-    </row>
-    <row r="381" spans="1:5">
-      <c r="A381" s="3" t="s">
-        <v>1886</v>
-      </c>
-      <c r="B381" s="15" t="s">
+      <c r="E381" s="15" t="s">
+        <v>1902</v>
+      </c>
+    </row>
+    <row r="382" spans="1:5" ht="30">
+      <c r="A382" s="3" t="s">
+        <v>1888</v>
+      </c>
+      <c r="B382" s="15" t="s">
         <v>1887</v>
       </c>
-      <c r="C381" s="15" t="s">
+      <c r="C382" s="15" t="s">
         <v>1894</v>
       </c>
-      <c r="D381" s="15" t="s">
+      <c r="D382" s="15" t="s">
         <v>1900</v>
       </c>
-      <c r="E381" s="15" t="s">
+      <c r="E382" s="15" t="s">
         <v>1903</v>
-      </c>
-    </row>
-    <row r="382" spans="1:5">
-      <c r="A382" s="3" t="s">
-        <v>1889</v>
-      </c>
-      <c r="B382" s="15" t="s">
-        <v>1888</v>
-      </c>
-      <c r="C382" s="15" t="s">
-        <v>1895</v>
-      </c>
-      <c r="D382" s="15" t="s">
-        <v>1901</v>
-      </c>
-      <c r="E382" s="15" t="s">
-        <v>1904</v>
       </c>
     </row>
     <row r="383" spans="1:5">
       <c r="A383" s="3" t="s">
-        <v>1907</v>
+        <v>1906</v>
       </c>
       <c r="B383" s="15" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="C383" s="15" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="D383" s="15" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
       <c r="E383" s="15" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="384" spans="1:5">
       <c r="A384" s="3" t="s">
+        <v>1907</v>
+      </c>
+      <c r="B384" s="15" t="s">
         <v>1908</v>
       </c>
-      <c r="B384" s="15" t="s">
-        <v>1909</v>
-      </c>
       <c r="C384" s="15" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="D384" s="15" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="E384" s="15" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
     </row>
   </sheetData>
@@ -13062,49 +13071,49 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="42.41796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="16" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>1770</v>
+        <v>1769</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
     </row>
     <row r="9" spans="1:1">
@@ -13119,12 +13128,12 @@
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
     </row>
   </sheetData>
@@ -13142,14 +13151,14 @@
       <selection pane="bottomLeft" activeCell="B252" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="44.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="44.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.83984375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="44.41796875" style="3"/>
-    <col min="3" max="3" width="50.26171875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="54.41796875" style="3" customWidth="1"/>
-    <col min="5" max="43" width="44.41796875" style="4"/>
-    <col min="44" max="16384" width="44.41796875" style="3"/>
+    <col min="1" max="1" width="16.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" style="3"/>
+    <col min="3" max="3" width="50.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="54.42578125" style="3" customWidth="1"/>
+    <col min="5" max="43" width="44.42578125" style="4"/>
+    <col min="44" max="16384" width="44.42578125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1">
@@ -13407,7 +13416,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="16" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A16" s="3" t="s">
         <v>68</v>
       </c>
@@ -13424,7 +13433,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="4" customFormat="1">
+    <row r="17" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A17" s="3" t="s">
         <v>73</v>
       </c>
@@ -13679,7 +13688,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="32" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A32" s="3" t="s">
         <v>148</v>
       </c>
@@ -13696,7 +13705,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="33" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A33" s="3" t="s">
         <v>153</v>
       </c>
@@ -13713,7 +13722,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="34" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A34" s="3" t="s">
         <v>158</v>
       </c>
@@ -13730,7 +13739,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="35" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A35" s="3" t="s">
         <v>163</v>
       </c>
@@ -13781,7 +13790,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="38" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A38" s="3" t="s">
         <v>178</v>
       </c>
@@ -13900,7 +13909,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="4" customFormat="1">
+    <row r="45" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A45" s="3" t="s">
         <v>213</v>
       </c>
@@ -14019,7 +14028,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="4" customFormat="1" ht="57.6">
+    <row r="52" spans="1:5" s="4" customFormat="1" ht="60">
       <c r="A52" s="3" t="s">
         <v>245</v>
       </c>
@@ -14036,7 +14045,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="53" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A53" s="3" t="s">
         <v>249</v>
       </c>
@@ -14359,7 +14368,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="72" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="72" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A72" s="3" t="s">
         <v>343</v>
       </c>
@@ -14376,7 +14385,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="73" spans="1:5" s="4" customFormat="1">
+    <row r="73" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A73" s="3" t="s">
         <v>348</v>
       </c>
@@ -14427,7 +14436,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="76" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="76" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A76" s="3" t="s">
         <v>361</v>
       </c>
@@ -14444,7 +14453,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="77" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="77" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A77" s="3" t="s">
         <v>366</v>
       </c>
@@ -14461,7 +14470,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="78" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="78" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A78" s="3" t="s">
         <v>371</v>
       </c>
@@ -14478,7 +14487,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="79" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="79" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A79" s="3" t="s">
         <v>375</v>
       </c>
@@ -14495,7 +14504,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="80" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="80" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A80" s="3" t="s">
         <v>380</v>
       </c>
@@ -14648,7 +14657,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="89" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="89" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A89" s="3" t="s">
         <v>423</v>
       </c>
@@ -14665,7 +14674,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="90" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="90" spans="1:5" s="4" customFormat="1" ht="60">
       <c r="A90" s="3" t="s">
         <v>428</v>
       </c>
@@ -14682,7 +14691,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="91" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="91" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A91" s="3" t="s">
         <v>433</v>
       </c>
@@ -14784,7 +14793,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="97" spans="1:5" s="4" customFormat="1">
+    <row r="97" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A97" s="3" t="s">
         <v>463</v>
       </c>
@@ -14869,7 +14878,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="102" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="102" spans="1:5" s="4" customFormat="1" ht="60">
       <c r="A102" s="3" t="s">
         <v>488</v>
       </c>
@@ -14937,7 +14946,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="106" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="106" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A106" s="3" t="s">
         <v>508</v>
       </c>
@@ -14954,7 +14963,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="107" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="107" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A107" s="3" t="s">
         <v>513</v>
       </c>
@@ -14971,7 +14980,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="108" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="108" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A108" s="3" t="s">
         <v>518</v>
       </c>
@@ -14988,7 +14997,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="109" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="109" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A109" s="3" t="s">
         <v>523</v>
       </c>
@@ -15005,7 +15014,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="110" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="110" spans="1:5" s="4" customFormat="1" ht="60">
       <c r="A110" s="3" t="s">
         <v>528</v>
       </c>
@@ -15022,7 +15031,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="111" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="111" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A111" s="3" t="s">
         <v>533</v>
       </c>
@@ -15039,7 +15048,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="112" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="112" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A112" s="3" t="s">
         <v>538</v>
       </c>
@@ -15056,7 +15065,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="113" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="113" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A113" s="3" t="s">
         <v>543</v>
       </c>
@@ -15073,7 +15082,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="114" spans="1:5" s="4" customFormat="1">
+    <row r="114" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A114" s="3" t="s">
         <v>548</v>
       </c>
@@ -15090,7 +15099,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="115" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="115" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A115" s="3" t="s">
         <v>553</v>
       </c>
@@ -15226,7 +15235,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="123" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="123" spans="1:5" s="4" customFormat="1" ht="60">
       <c r="A123" s="3" t="s">
         <v>593</v>
       </c>
@@ -15328,7 +15337,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="129" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="129" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A129" s="3" t="s">
         <v>623</v>
       </c>
@@ -15379,7 +15388,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="132" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="132" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A132" s="3" t="s">
         <v>638</v>
       </c>
@@ -15396,7 +15405,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="133" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="133" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A133" s="3" t="s">
         <v>643</v>
       </c>
@@ -15413,7 +15422,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="134" spans="1:5" s="4" customFormat="1" ht="72">
+    <row r="134" spans="1:5" s="4" customFormat="1" ht="75">
       <c r="A134" s="3" t="s">
         <v>648</v>
       </c>
@@ -15481,7 +15490,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="138" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="138" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A138" s="3" t="s">
         <v>668</v>
       </c>
@@ -15498,7 +15507,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="139" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="139" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A139" s="3" t="s">
         <v>673</v>
       </c>
@@ -15515,7 +15524,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="140" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="140" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A140" s="3" t="s">
         <v>678</v>
       </c>
@@ -15532,7 +15541,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="141" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="141" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A141" s="3" t="s">
         <v>683</v>
       </c>
@@ -15566,7 +15575,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="143" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="143" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A143" s="3" t="s">
         <v>693</v>
       </c>
@@ -15583,7 +15592,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="144" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="144" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A144" s="3" t="s">
         <v>698</v>
       </c>
@@ -15651,7 +15660,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="148" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="148" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A148" s="3" t="s">
         <v>718</v>
       </c>
@@ -15668,7 +15677,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="149" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="149" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A149" s="3" t="s">
         <v>723</v>
       </c>
@@ -15702,7 +15711,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="151" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="151" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A151" s="3" t="s">
         <v>733</v>
       </c>
@@ -15736,7 +15745,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="153" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="153" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A153" s="3" t="s">
         <v>743</v>
       </c>
@@ -15753,7 +15762,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="154" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="154" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A154" s="3" t="s">
         <v>748</v>
       </c>
@@ -15770,7 +15779,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="155" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="155" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A155" s="3" t="s">
         <v>753</v>
       </c>
@@ -15787,7 +15796,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="156" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="156" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A156" s="3" t="s">
         <v>758</v>
       </c>
@@ -15804,7 +15813,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="157" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="157" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A157" s="3" t="s">
         <v>763</v>
       </c>
@@ -15838,7 +15847,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="159" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="159" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A159" s="3" t="s">
         <v>773</v>
       </c>
@@ -15872,7 +15881,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="161" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="161" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A161" s="3" t="s">
         <v>783</v>
       </c>
@@ -15889,7 +15898,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="162" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="162" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A162" s="3" t="s">
         <v>788</v>
       </c>
@@ -15906,7 +15915,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="163" spans="1:5" s="4" customFormat="1" ht="57.6">
+    <row r="163" spans="1:5" s="4" customFormat="1" ht="60">
       <c r="A163" s="3" t="s">
         <v>793</v>
       </c>
@@ -15923,7 +15932,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="164" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="164" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A164" s="3" t="s">
         <v>798</v>
       </c>
@@ -15957,7 +15966,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="166" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="166" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A166" s="3" t="s">
         <v>808</v>
       </c>
@@ -15974,7 +15983,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="167" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="167" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A167" s="3" t="s">
         <v>813</v>
       </c>
@@ -16008,7 +16017,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="169" spans="1:5" s="4" customFormat="1" ht="57.6">
+    <row r="169" spans="1:5" s="4" customFormat="1" ht="75">
       <c r="A169" s="3" t="s">
         <v>823</v>
       </c>
@@ -16025,7 +16034,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="170" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="170" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A170" s="3" t="s">
         <v>828</v>
       </c>
@@ -16042,7 +16051,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="171" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="171" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A171" s="3" t="s">
         <v>833</v>
       </c>
@@ -16059,7 +16068,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="172" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="172" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A172" s="3" t="s">
         <v>838</v>
       </c>
@@ -16076,7 +16085,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="173" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="173" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A173" s="3" t="s">
         <v>843</v>
       </c>
@@ -16144,7 +16153,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="177" spans="1:5" s="4" customFormat="1">
+    <row r="177" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A177" s="3" t="s">
         <v>863</v>
       </c>
@@ -16161,7 +16170,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="178" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="178" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A178" s="3" t="s">
         <v>868</v>
       </c>
@@ -16195,7 +16204,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="180" spans="1:5" s="4" customFormat="1" ht="57.6">
+    <row r="180" spans="1:5" s="4" customFormat="1" ht="75">
       <c r="A180" s="3" t="s">
         <v>878</v>
       </c>
@@ -16229,7 +16238,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="182" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="182" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A182" s="3" t="s">
         <v>888</v>
       </c>
@@ -16246,7 +16255,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="183" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="183" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A183" s="3" t="s">
         <v>893</v>
       </c>
@@ -16280,7 +16289,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="185" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="185" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A185" s="3" t="s">
         <v>903</v>
       </c>
@@ -16314,7 +16323,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="187" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="187" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A187" s="3" t="s">
         <v>913</v>
       </c>
@@ -16331,7 +16340,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="188" spans="1:5" s="4" customFormat="1" ht="115.2">
+    <row r="188" spans="1:5" s="4" customFormat="1" ht="135">
       <c r="A188" s="3" t="s">
         <v>918</v>
       </c>
@@ -16348,7 +16357,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="189" spans="1:5" s="4" customFormat="1" ht="72">
+    <row r="189" spans="1:5" s="4" customFormat="1" ht="75">
       <c r="A189" s="3" t="s">
         <v>923</v>
       </c>
@@ -16365,7 +16374,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="190" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="190" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A190" s="3" t="s">
         <v>928</v>
       </c>
@@ -16382,7 +16391,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="191" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="191" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A191" s="3" t="s">
         <v>933</v>
       </c>
@@ -16399,7 +16408,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="192" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="192" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A192" s="3" t="s">
         <v>938</v>
       </c>
@@ -16416,7 +16425,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="193" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="193" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A193" s="3" t="s">
         <v>943</v>
       </c>
@@ -16433,7 +16442,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="194" spans="1:5" s="4" customFormat="1" ht="100.8">
+    <row r="194" spans="1:5" s="4" customFormat="1" ht="105">
       <c r="A194" s="3" t="s">
         <v>948</v>
       </c>
@@ -16450,7 +16459,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="195" spans="1:5" s="4" customFormat="1" ht="86.4">
+    <row r="195" spans="1:5" s="4" customFormat="1" ht="105">
       <c r="A195" s="3" t="s">
         <v>953</v>
       </c>
@@ -16467,7 +16476,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="196" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="196" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A196" s="3" t="s">
         <v>958</v>
       </c>
@@ -16484,7 +16493,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="197" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="197" spans="1:5" s="4" customFormat="1" ht="60">
       <c r="A197" s="3" t="s">
         <v>963</v>
       </c>
@@ -16501,7 +16510,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="198" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="198" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A198" s="3" t="s">
         <v>968</v>
       </c>
@@ -16552,7 +16561,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="201" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="201" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A201" s="3" t="s">
         <v>983</v>
       </c>
@@ -16637,7 +16646,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="206" spans="1:5" s="4" customFormat="1">
+    <row r="206" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A206" s="3" t="s">
         <v>1008</v>
       </c>
@@ -16654,7 +16663,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="207" spans="1:5" s="4" customFormat="1">
+    <row r="207" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A207" s="3" t="s">
         <v>1013</v>
       </c>
@@ -16688,7 +16697,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="209" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="209" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A209" s="3" t="s">
         <v>1023</v>
       </c>
@@ -16705,7 +16714,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="210" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="210" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A210" s="3" t="s">
         <v>1028</v>
       </c>
@@ -16722,7 +16731,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="211" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="211" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A211" s="3" t="s">
         <v>1033</v>
       </c>
@@ -16756,7 +16765,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="213" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="213" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A213" s="3" t="s">
         <v>1043</v>
       </c>
@@ -16773,7 +16782,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="214" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="214" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A214" s="3" t="s">
         <v>1048</v>
       </c>
@@ -16790,7 +16799,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="215" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="215" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A215" s="3" t="s">
         <v>1053</v>
       </c>
@@ -16807,7 +16816,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="216" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="216" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A216" s="3" t="s">
         <v>1058</v>
       </c>
@@ -16824,7 +16833,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="217" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="217" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A217" s="3" t="s">
         <v>1063</v>
       </c>
@@ -16994,7 +17003,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="227" spans="1:5" s="4" customFormat="1">
+    <row r="227" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A227" s="3" t="s">
         <v>1111</v>
       </c>
@@ -17096,7 +17105,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="233" spans="1:5" s="4" customFormat="1" ht="43" customHeight="1">
+    <row r="233" spans="1:5" s="4" customFormat="1" ht="42.95" customHeight="1">
       <c r="A233" s="3" t="s">
         <v>1141</v>
       </c>
@@ -17113,7 +17122,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="234" spans="1:5" s="4" customFormat="1">
+    <row r="234" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A234" s="3" t="s">
         <v>1146</v>
       </c>
@@ -17147,7 +17156,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="236" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="236" spans="1:5" s="4" customFormat="1" ht="60">
       <c r="A236" s="3" t="s">
         <v>1156</v>
       </c>
@@ -17164,7 +17173,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="237" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="237" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A237" s="3" t="s">
         <v>1160</v>
       </c>
@@ -17198,7 +17207,7 @@
         <v>1169</v>
       </c>
     </row>
-    <row r="239" spans="1:5" s="4" customFormat="1">
+    <row r="239" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A239" s="3" t="s">
         <v>1170</v>
       </c>
@@ -17215,7 +17224,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="240" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="240" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A240" s="3" t="s">
         <v>1175</v>
       </c>
@@ -17283,7 +17292,7 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="244" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="244" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A244" s="3" t="s">
         <v>1195</v>
       </c>
@@ -17300,7 +17309,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="245" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="245" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A245" s="3" t="s">
         <v>1200</v>
       </c>
@@ -17317,7 +17326,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="246" spans="1:5" s="4" customFormat="1" ht="43.2">
+    <row r="246" spans="1:5" s="4" customFormat="1" ht="45">
       <c r="A246" s="3" t="s">
         <v>1205</v>
       </c>
@@ -17351,7 +17360,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="248" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="248" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A248" s="3" t="s">
         <v>1215</v>
       </c>
@@ -17368,7 +17377,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="249" spans="1:5" s="4" customFormat="1" ht="28.8">
+    <row r="249" spans="1:5" s="4" customFormat="1" ht="30">
       <c r="A249" s="3" t="s">
         <v>1220</v>
       </c>
@@ -17407,7 +17416,7 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="78" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
change MOSV to MOV in column titles for DESC_03 2 and 6
</commit_message>
<xml_diff>
--- a/Demo_Datasets/ES/Multi-Lingual Phrases - En Fr Es Pt.xlsx
+++ b/Demo_Datasets/ES/Multi-Lingual Phrases - En Fr Es Pt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mia\Biostat Global Dropbox\Mia Yu\My Github Repost\missvcqiR\Demo_Datasets\ES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9189F3-73DA-4734-8D13-75220CB91545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588AA874-CF27-4A85-8BDB-4D9F85D25A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{50234D21-0CB7-4831-B1A7-1E2C296C3191}"/>
   </bookViews>
@@ -6197,7 +6197,7 @@
     <t>Relacionado con Cuidadores: Razones de la OPV de los encuestados que eran elegibles para recibir más de 1 dosis</t>
   </si>
   <si>
-    <t>Update following strings: OS_225, OS_142, OS_148,  OS_149, OS_160, OS_384, OS_385, OS_386, OS_387, OS_388 on 2024-03-11</t>
+    <t>Update following strings: OS_225, OS_142, OS_148,  OS_149, OS_160, OS_226, OS_227, OS_228, OS_229, OS_384, OS_385, OS_386, OS_387, OS_388 on 2024-03-11</t>
   </si>
 </sst>
 </file>
@@ -6696,8 +6696,8 @@
   <dimension ref="A1:AQ389"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E150" sqref="B150:E150"/>
+      <pane ySplit="1" topLeftCell="A213" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B232" sqref="B232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="44.3984375" defaultRowHeight="14.25"/>
@@ -10556,16 +10556,16 @@
       <c r="A227" s="3" t="s">
         <v>1111</v>
       </c>
-      <c r="B227" s="6" t="s">
-        <v>1759</v>
-      </c>
-      <c r="C227" s="7" t="s">
+      <c r="B227" s="1" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C227" s="17" t="s">
         <v>1113</v>
       </c>
-      <c r="D227" s="6" t="s">
+      <c r="D227" s="1" t="s">
         <v>1114</v>
       </c>
-      <c r="E227" s="6" t="s">
+      <c r="E227" s="1" t="s">
         <v>1115</v>
       </c>
     </row>
@@ -10573,16 +10573,16 @@
       <c r="A228" s="3" t="s">
         <v>1116</v>
       </c>
-      <c r="B228" s="6" t="s">
-        <v>1760</v>
-      </c>
-      <c r="C228" s="7" t="s">
+      <c r="B228" s="1" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C228" s="17" t="s">
         <v>1118</v>
       </c>
-      <c r="D228" s="6" t="s">
+      <c r="D228" s="1" t="s">
         <v>1119</v>
       </c>
-      <c r="E228" s="6" t="s">
+      <c r="E228" s="1" t="s">
         <v>1120</v>
       </c>
     </row>
@@ -10590,16 +10590,16 @@
       <c r="A229" s="3" t="s">
         <v>1121</v>
       </c>
-      <c r="B229" s="6" t="s">
-        <v>1761</v>
-      </c>
-      <c r="C229" s="7" t="s">
+      <c r="B229" s="1" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C229" s="17" t="s">
         <v>1123</v>
       </c>
-      <c r="D229" s="6" t="s">
+      <c r="D229" s="1" t="s">
         <v>1124</v>
       </c>
-      <c r="E229" s="6" t="s">
+      <c r="E229" s="1" t="s">
         <v>1125</v>
       </c>
     </row>
@@ -10607,16 +10607,16 @@
       <c r="A230" s="3" t="s">
         <v>1126</v>
       </c>
-      <c r="B230" s="6" t="s">
-        <v>1762</v>
-      </c>
-      <c r="C230" s="7" t="s">
+      <c r="B230" s="1" t="s">
+        <v>1127</v>
+      </c>
+      <c r="C230" s="17" t="s">
         <v>1128</v>
       </c>
-      <c r="D230" s="6" t="s">
+      <c r="D230" s="1" t="s">
         <v>1129</v>
       </c>
-      <c r="E230" s="6" t="s">
+      <c r="E230" s="1" t="s">
         <v>1130</v>
       </c>
     </row>
@@ -24239,7 +24239,7 @@
   <dimension ref="A2:A4"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>